<commit_message>
Updated literature with ambient occlusion & thesis introduction.
</commit_message>
<xml_diff>
--- a/literature.xlsx
+++ b/literature.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Stacknit/Github/thesis/literature/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stacknit\Desktop\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="825" yWindow="465" windowWidth="25605" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
   <si>
     <t>Name</t>
   </si>
@@ -230,9 +230,6 @@
     <t>Scattering und Gathering gemischt</t>
   </si>
   <si>
-    <t>Mapping particle position to grid cell contributions -&gt; ÄHNLICH  ZU MEINER ARBERIT</t>
-  </si>
-  <si>
     <t>Gather: weniger atomics, mehr memory transact. + gpu arch. abhängig,</t>
   </si>
   <si>
@@ -302,9 +299,6 @@
     <t>Dynamic Ambient Occlusion</t>
   </si>
   <si>
-    <t>Voxelization -&gt; Motiviert Gathering Ansatz</t>
-  </si>
-  <si>
     <t>Precomputed Ambient Occlusion</t>
   </si>
   <si>
@@ -323,17 +317,95 @@
     <t>Voxelisierung -&gt; Sortierverfahren</t>
   </si>
   <si>
-    <t>Voxelization -&gt; Grid sollte sortiert sein</t>
-  </si>
-  <si>
     <t xml:space="preserve">Radius Nearest Neighbor Search + Vergleich Sortierverfahren + Vergleich Software </t>
+  </si>
+  <si>
+    <t>Bezug</t>
+  </si>
+  <si>
+    <t>Finding next gen: CryEngine 2</t>
+  </si>
+  <si>
+    <t>Mittring</t>
+  </si>
+  <si>
+    <t>Screen Space Ambient Occlusion</t>
+  </si>
+  <si>
+    <t>less accurate, less expensive</t>
+  </si>
+  <si>
+    <t>Image-space horizon-based ambient occlusion</t>
+  </si>
+  <si>
+    <t>Bavoil</t>
+  </si>
+  <si>
+    <t>Horizon Based Ambient Occlusion</t>
+  </si>
+  <si>
+    <t>Mapping particle position to grid cell contributions</t>
+  </si>
+  <si>
+    <t>Voxelization -&gt; Motiviert Gathering</t>
+  </si>
+  <si>
+    <t>Voxelization -&gt; Grid sortieren</t>
+  </si>
+  <si>
+    <t>Partikel -&gt; Grid mit Gathering</t>
+  </si>
+  <si>
+    <t>Datenstruktur für Partikelsuche</t>
+  </si>
+  <si>
+    <t>Partikelsuche ohne Datenstruktur</t>
+  </si>
+  <si>
+    <t>Voxelisieren Partikel, aber wir suchen keine Oberfläche</t>
+  </si>
+  <si>
+    <t>Partikelberechnungen auf GPU</t>
+  </si>
+  <si>
+    <t>Partikel -&gt; Grid</t>
+  </si>
+  <si>
+    <t>Partikelsuche + Sortierverfahren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partikelsuche mit Datenstrukturen </t>
+  </si>
+  <si>
+    <t>Partikel AO mittels Voxel</t>
+  </si>
+  <si>
+    <t>Rartikel AO mittels Voxel  + Cone Tracing</t>
+  </si>
+  <si>
+    <t>Stable SSAO in Battlefield 3 with Selective Temporal Filtering</t>
+  </si>
+  <si>
+    <t>Advanced Ambient Occlusion Methods for Modern Games</t>
+  </si>
+  <si>
+    <t>Tatarinov</t>
+  </si>
+  <si>
+    <t>HBAO without flickering</t>
+  </si>
+  <si>
+    <t>Second Depth buffer for moving objects</t>
+  </si>
+  <si>
+    <t>HBAO+ &amp; Voxel AO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -422,6 +494,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -453,7 +531,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -484,10 +562,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -496,19 +570,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -777,25 +859,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC28"/>
+  <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="80.83203125" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="80.875" customWidth="1"/>
+    <col min="2" max="2" width="5.625" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
     <col min="4" max="4" width="76.5" customWidth="1"/>
-    <col min="5" max="5" width="54.33203125" customWidth="1"/>
-    <col min="6" max="6" width="47.1640625" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="54.375" customWidth="1"/>
+    <col min="6" max="6" width="58.5" customWidth="1"/>
+    <col min="7" max="7" width="30.25" customWidth="1"/>
+    <col min="8" max="8" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -817,13 +899,16 @@
       <c r="G1" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="H1" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -834,19 +919,22 @@
         <v>11</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="H4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -860,16 +948,19 @@
         <v>64</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -880,16 +971,19 @@
         <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="H6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -900,39 +994,41 @@
         <v>13</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="19"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -946,36 +1042,38 @@
         <v>16</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="21"/>
-      <c r="AC8" s="21"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
+      <c r="X8" s="19"/>
+      <c r="Y8" s="19"/>
+      <c r="Z8" s="19"/>
+      <c r="AA8" s="19"/>
+      <c r="AB8" s="19"/>
+      <c r="AC8" s="19"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -986,37 +1084,39 @@
         <v>18</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="21"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+      <c r="X9" s="19"/>
+      <c r="Y9" s="19"/>
+      <c r="Z9" s="19"/>
+      <c r="AA9" s="19"/>
+      <c r="AB9" s="19"/>
+      <c r="AC9" s="19"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1027,39 +1127,41 @@
         <v>20</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
-      <c r="AC10" s="21"/>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="19"/>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="19"/>
+      <c r="AB10" s="19"/>
+      <c r="AC10" s="19"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>30</v>
       </c>
@@ -1069,40 +1171,42 @@
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="21" t="s">
+      <c r="D11" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="19" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="21"/>
-      <c r="AA11" s="21"/>
-      <c r="AB11" s="21"/>
-      <c r="AC11" s="21"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="19"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -1112,51 +1216,53 @@
       <c r="C12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="21"/>
-      <c r="W12" s="21"/>
-      <c r="X12" s="21"/>
-      <c r="Y12" s="21"/>
-      <c r="Z12" s="21"/>
-      <c r="AA12" s="21"/>
-      <c r="AB12" s="21"/>
-      <c r="AC12" s="21"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="G12" s="19"/>
+      <c r="H12" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="19"/>
+      <c r="AC12" s="19"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="23">
         <v>2014</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>51</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>65</v>
@@ -1164,33 +1270,35 @@
       <c r="F13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
-      <c r="X13" s="21"/>
-      <c r="Y13" s="21"/>
-      <c r="Z13" s="21"/>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="21"/>
-      <c r="AC13" s="21"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="G13" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
+      <c r="AC13" s="19"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>52</v>
       </c>
@@ -1201,38 +1309,40 @@
         <v>53</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" t="s">
         <v>72</v>
       </c>
-      <c r="F14" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="21"/>
-      <c r="X14" s="21"/>
-      <c r="Y14" s="21"/>
-      <c r="Z14" s="21"/>
-      <c r="AA14" s="21"/>
-      <c r="AB14" s="21"/>
-      <c r="AC14" s="21"/>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="H14" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
+      <c r="AC14" s="19"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>21</v>
       </c>
@@ -1242,31 +1352,31 @@
       <c r="C15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="17"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="10">
         <v>2006</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>44</v>
       </c>
@@ -1276,7 +1386,7 @@
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>22</v>
       </c>
@@ -1289,10 +1399,10 @@
       <c r="D19" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>25</v>
       </c>
@@ -1305,12 +1415,12 @@
       <c r="D20" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" s="14">
         <v>2007</v>
@@ -1319,28 +1429,28 @@
         <v>32</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="22"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="24" t="s">
-        <v>88</v>
+      <c r="F21" s="20"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>87</v>
       </c>
       <c r="B22" s="6">
         <v>2005</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
@@ -1353,23 +1463,23 @@
       <c r="D23" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="23" t="s">
-        <v>82</v>
+      <c r="F23" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="G23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1379,11 +1489,11 @@
       <c r="C25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -1393,11 +1503,11 @@
       <c r="C26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
@@ -1407,25 +1517,88 @@
       <c r="C27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="7">
+        <v>2007</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="7">
+        <v>2008</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" s="7">
+        <v>2012</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="7">
+        <v>2016</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" t="s">
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>